<commit_message>
Started Clipping Signed-off-by: Jack <jack.patterson@students.ittralee.ie>
</commit_message>
<xml_diff>
--- a/J_Graphics_XL.xlsx
+++ b/J_Graphics_XL.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t00217640\Desktop\Computer-Graphics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t00217640\Desktop\CG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03594F13-4152-4C6C-9A4E-43FDD427EDC9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51519C21-133C-4BA5-A4A8-A037FB630AF9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{33A02D27-0B54-443A-8ABA-B568FEBCC2A9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{33A02D27-0B54-443A-8ABA-B568FEBCC2A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="VerticesFaces" sheetId="2" r:id="rId2"/>
     <sheet name="Textures" sheetId="3" r:id="rId3"/>
+    <sheet name="Clipping" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -581,12 +582,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -595,6 +590,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2413,11 +2414,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="57"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="55"/>
       <c r="E1"/>
       <c r="F1"/>
       <c r="G1" s="4"/>
@@ -2427,24 +2428,24 @@
       <c r="K1" s="4"/>
       <c r="L1"/>
       <c r="M1"/>
-      <c r="V1" s="54" t="s">
+      <c r="V1" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="AI1" s="54" t="s">
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="AI1" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="AJ1" s="54"/>
-      <c r="AK1" s="54"/>
-      <c r="AL1" s="54"/>
-      <c r="AM1" s="54"/>
-      <c r="AN1" s="54"/>
-      <c r="AU1" s="54" t="s">
+      <c r="AJ1" s="56"/>
+      <c r="AK1" s="56"/>
+      <c r="AL1" s="56"/>
+      <c r="AM1" s="56"/>
+      <c r="AN1" s="56"/>
+      <c r="AU1" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="AV1" s="54"/>
-      <c r="AW1" s="54"/>
+      <c r="AV1" s="56"/>
+      <c r="AW1" s="56"/>
     </row>
     <row r="2" spans="1:49" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="46" t="s">
@@ -2521,26 +2522,26 @@
       <c r="K3"/>
       <c r="L3"/>
       <c r="M3"/>
-      <c r="V3" s="54" t="s">
+      <c r="V3" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="W3" s="54"/>
-      <c r="X3" s="54"/>
-      <c r="AI3" s="54" t="s">
+      <c r="W3" s="56"/>
+      <c r="X3" s="56"/>
+      <c r="AI3" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="AJ3" s="54"/>
-      <c r="AK3" s="54"/>
-      <c r="AL3" s="53" t="s">
+      <c r="AJ3" s="56"/>
+      <c r="AK3" s="56"/>
+      <c r="AL3" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="AM3" s="53"/>
-      <c r="AN3" s="53"/>
-      <c r="AU3" s="53" t="s">
+      <c r="AM3" s="57"/>
+      <c r="AN3" s="57"/>
+      <c r="AU3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="AV3" s="53"/>
-      <c r="AW3" s="53"/>
+      <c r="AV3" s="57"/>
+      <c r="AW3" s="57"/>
     </row>
     <row r="4" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A4" s="48">
@@ -2646,11 +2647,11 @@
       <c r="AN5" s="14">
         <v>4</v>
       </c>
-      <c r="AU5" s="53" t="s">
+      <c r="AU5" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="AV5" s="53"/>
-      <c r="AW5" s="53"/>
+      <c r="AV5" s="57"/>
+      <c r="AW5" s="57"/>
     </row>
     <row r="6" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A6" s="48">
@@ -2680,11 +2681,11 @@
       <c r="X6" s="14">
         <v>6</v>
       </c>
-      <c r="AI6" s="53" t="s">
+      <c r="AI6" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="AJ6" s="53"/>
-      <c r="AK6" s="53"/>
+      <c r="AJ6" s="57"/>
+      <c r="AK6" s="57"/>
       <c r="AL6">
         <v>4</v>
       </c>
@@ -2750,11 +2751,11 @@
       <c r="AN7">
         <v>17</v>
       </c>
-      <c r="AU7" s="53" t="s">
+      <c r="AU7" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="AV7" s="53"/>
-      <c r="AW7" s="53"/>
+      <c r="AV7" s="57"/>
+      <c r="AW7" s="57"/>
     </row>
     <row r="8" spans="1:49" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="48">
@@ -2859,11 +2860,11 @@
       <c r="AN9">
         <v>8</v>
       </c>
-      <c r="AU9" s="53" t="s">
+      <c r="AU9" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="AV9" s="53"/>
-      <c r="AW9" s="53"/>
+      <c r="AV9" s="57"/>
+      <c r="AW9" s="57"/>
     </row>
     <row r="10" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="48">
@@ -2945,16 +2946,16 @@
       <c r="X11" s="14">
         <v>7</v>
       </c>
-      <c r="AI11" s="53" t="s">
+      <c r="AI11" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="AJ11" s="53"/>
-      <c r="AK11" s="53"/>
-      <c r="AU11" s="53" t="s">
+      <c r="AJ11" s="57"/>
+      <c r="AK11" s="57"/>
+      <c r="AU11" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="AV11" s="53"/>
-      <c r="AW11" s="53"/>
+      <c r="AV11" s="57"/>
+      <c r="AW11" s="57"/>
     </row>
     <row r="12" spans="1:49" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="48">
@@ -2975,11 +2976,11 @@
       <c r="J12"/>
       <c r="K12" s="26"/>
       <c r="L12"/>
-      <c r="V12" s="53" t="s">
+      <c r="V12" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="W12" s="53"/>
-      <c r="X12" s="53"/>
+      <c r="W12" s="57"/>
+      <c r="X12" s="57"/>
       <c r="AI12" s="14">
         <v>13</v>
       </c>
@@ -3036,11 +3037,11 @@
       <c r="AK13" s="14">
         <v>3</v>
       </c>
-      <c r="AU13" s="53" t="s">
+      <c r="AU13" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="AV13" s="53"/>
-      <c r="AW13" s="53"/>
+      <c r="AV13" s="57"/>
+      <c r="AW13" s="57"/>
     </row>
     <row r="14" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A14" s="48">
@@ -3594,13 +3595,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="V1:X1"/>
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="V12:X12"/>
-    <mergeCell ref="AI3:AK3"/>
-    <mergeCell ref="AI6:AK6"/>
-    <mergeCell ref="AI11:AK11"/>
     <mergeCell ref="AU13:AW13"/>
     <mergeCell ref="AU11:AW11"/>
     <mergeCell ref="AL3:AN3"/>
@@ -3610,6 +3604,13 @@
     <mergeCell ref="AU5:AW5"/>
     <mergeCell ref="AU9:AW9"/>
     <mergeCell ref="AU7:AW7"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="V12:X12"/>
+    <mergeCell ref="AI3:AK3"/>
+    <mergeCell ref="AI6:AK6"/>
+    <mergeCell ref="AI11:AK11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3620,7 +3621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE6656B1-986B-4CD6-84BB-FEF14906E93B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
@@ -3629,4 +3630,75 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF1D3BE0-E755-4AFA-AFA4-25C6C8DEFFEC}">
+  <dimension ref="E2:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>